<commit_message>
Rettelse af PwThat/phi ligning + startet på stød
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/techdata_dors_3_overlap.xlsx
+++ b/examples/Abatement/Data/techdata_dors_3_overlap.xlsx
@@ -531,7 +531,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F3" sqref="F3"/>
+      <selection pane="topRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +619,7 @@
         <v>0.01</v>
       </c>
       <c r="I2">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J2">
         <v>0.2</v>
@@ -642,7 +642,7 @@
         <v>0.02</v>
       </c>
       <c r="I3">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>0.02</v>
       </c>
       <c r="I4">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="J4">
         <v>0.2</v>

</xml_diff>